<commit_message>
modification des données brutes
</commit_message>
<xml_diff>
--- a/data/raw/Excel - trafic routier.xlsx
+++ b/data/raw/Excel - trafic routier.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\serietemporelle\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8A45CC-2AD1-4386-8009-9D1189B6980B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EACAFAB-4966-4C08-A44F-C569142F5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,18 @@
     <sheet name="caractéristiques" sheetId="2" r:id="rId2"/>
     <sheet name="codes" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">valeurs_mensuelles!$B$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">valeurs_mensuelles!$C$2:$KC$2</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">valeurs_mensuelles!$B$2</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">valeurs_mensuelles!$C$2:$KC$2</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="339">
   <si>
     <t>Libellé</t>
   </si>
@@ -1045,8 +1051,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1107,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1121,6 +1128,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1464,877 +1474,880 @@
   <dimension ref="A1:KC2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:289" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="O1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="P1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="Q1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="S1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="T1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="U1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="W1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="X1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="Y1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="Z1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AA1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AB1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AC1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AD1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AE1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AF1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AG1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AH1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AI1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AK1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AL1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AM1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AN1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AO1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AP1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AQ1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AR1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AS1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AT1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AU1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AV1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AW1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AX1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="AY1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="AZ1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BA1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BB1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BC1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BD1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BE1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BF1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BG1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BH1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BI1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BK1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BL1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BM1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BN1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BO1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BP1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BQ1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BR1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BS1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BT1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BU1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BV1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BW1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="BX1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="BY1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="BZ1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CA1" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CB1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CC1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CD1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CE1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CF1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CG1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CH1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CI1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CJ1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CK1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CL1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CM1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CN1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CO1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CP1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CQ1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CR1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CS1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="CT1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="CU1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="CV1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="CW1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="CX1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="CY1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="CZ1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DA1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DB1" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DC1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DD1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DE1" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DF1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="2" t="s">
+      <c r="DG1" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DH1" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DI1" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DJ1" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DK1" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DL1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DM1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DN1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DO1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DP1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DQ1" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DR1" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="DS1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="DT1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="DU1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="DV1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="DW1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="DX1" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" s="2" t="s">
+      <c r="DY1" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" s="2" t="s">
+      <c r="DZ1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" s="2" t="s">
+      <c r="EA1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" s="2" t="s">
+      <c r="EB1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" s="2" t="s">
+      <c r="EC1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="EF1" s="2" t="s">
+      <c r="ED1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="EG1" s="2" t="s">
+      <c r="EE1" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="EH1" s="2" t="s">
+      <c r="EF1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="EI1" s="2" t="s">
+      <c r="EG1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" s="2" t="s">
+      <c r="EH1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" s="2" t="s">
+      <c r="EI1" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" s="2" t="s">
+      <c r="EJ1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" s="2" t="s">
+      <c r="EK1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" s="2" t="s">
+      <c r="EL1" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="EO1" s="2" t="s">
+      <c r="EM1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="EP1" s="2" t="s">
+      <c r="EN1" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="EQ1" s="2" t="s">
+      <c r="EO1" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="ER1" s="2" t="s">
+      <c r="EP1" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="ES1" s="2" t="s">
+      <c r="EQ1" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="ET1" s="2" t="s">
+      <c r="ER1" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="EU1" s="2" t="s">
+      <c r="ES1" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="EV1" s="2" t="s">
+      <c r="ET1" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="EW1" s="2" t="s">
+      <c r="EU1" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="EX1" s="2" t="s">
+      <c r="EV1" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="EY1" s="2" t="s">
+      <c r="EW1" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="EZ1" s="2" t="s">
+      <c r="EX1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="FA1" s="2" t="s">
+      <c r="EY1" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="FB1" s="2" t="s">
+      <c r="EZ1" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="FC1" s="2" t="s">
+      <c r="FA1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="FD1" s="2" t="s">
+      <c r="FB1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="FE1" s="2" t="s">
+      <c r="FC1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="FF1" s="2" t="s">
+      <c r="FD1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="FG1" s="2" t="s">
+      <c r="FE1" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="FH1" s="2" t="s">
+      <c r="FF1" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="FI1" s="2" t="s">
+      <c r="FG1" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="FJ1" s="2" t="s">
+      <c r="FH1" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="FK1" s="2" t="s">
+      <c r="FI1" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="FL1" s="2" t="s">
+      <c r="FJ1" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="FM1" s="2" t="s">
+      <c r="FK1" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="FN1" s="2" t="s">
+      <c r="FL1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="FO1" s="2" t="s">
+      <c r="FM1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="FP1" s="2" t="s">
+      <c r="FN1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="FQ1" s="2" t="s">
+      <c r="FO1" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="FR1" s="2" t="s">
+      <c r="FP1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="FS1" s="2" t="s">
+      <c r="FQ1" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="FT1" s="2" t="s">
+      <c r="FR1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="FU1" s="2" t="s">
+      <c r="FS1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="FV1" s="2" t="s">
+      <c r="FT1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="FW1" s="2" t="s">
+      <c r="FU1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="FX1" s="2" t="s">
+      <c r="FV1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="FY1" s="2" t="s">
+      <c r="FW1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="FZ1" s="2" t="s">
+      <c r="FX1" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="GA1" s="2" t="s">
+      <c r="FY1" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="GB1" s="2" t="s">
+      <c r="FZ1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="GC1" s="2" t="s">
+      <c r="GA1" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="GD1" s="2" t="s">
+      <c r="GB1" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="GE1" s="2" t="s">
+      <c r="GC1" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="GF1" s="2" t="s">
+      <c r="GD1" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="GG1" s="2" t="s">
+      <c r="GE1" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="GH1" s="2" t="s">
+      <c r="GF1" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="GI1" s="2" t="s">
+      <c r="GG1" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="GJ1" s="2" t="s">
+      <c r="GH1" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="GK1" s="2" t="s">
+      <c r="GI1" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="GL1" s="2" t="s">
+      <c r="GJ1" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="GM1" s="2" t="s">
+      <c r="GK1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="GN1" s="2" t="s">
+      <c r="GL1" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="GO1" s="2" t="s">
+      <c r="GM1" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="GP1" s="2" t="s">
+      <c r="GN1" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="GQ1" s="2" t="s">
+      <c r="GO1" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="GR1" s="2" t="s">
+      <c r="GP1" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="GS1" s="2" t="s">
+      <c r="GQ1" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="GT1" s="2" t="s">
+      <c r="GR1" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="GU1" s="2" t="s">
+      <c r="GS1" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="GV1" s="2" t="s">
+      <c r="GT1" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="GW1" s="2" t="s">
+      <c r="GU1" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="GX1" s="2" t="s">
+      <c r="GV1" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="GY1" s="2" t="s">
+      <c r="GW1" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="GZ1" s="2" t="s">
+      <c r="GX1" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="HA1" s="2" t="s">
+      <c r="GY1" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="HB1" s="2" t="s">
+      <c r="GZ1" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="HC1" s="2" t="s">
+      <c r="HA1" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="HD1" s="2" t="s">
+      <c r="HB1" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="HE1" s="2" t="s">
+      <c r="HC1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="HF1" s="2" t="s">
+      <c r="HD1" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="HG1" s="2" t="s">
+      <c r="HE1" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="HH1" s="2" t="s">
+      <c r="HF1" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="HI1" s="2" t="s">
+      <c r="HG1" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="HJ1" s="2" t="s">
+      <c r="HH1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="HK1" s="2" t="s">
+      <c r="HI1" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="HL1" s="2" t="s">
+      <c r="HJ1" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="HM1" s="2" t="s">
+      <c r="HK1" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="HN1" s="2" t="s">
+      <c r="HL1" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="HO1" s="2" t="s">
+      <c r="HM1" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="HP1" s="2" t="s">
+      <c r="HN1" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="HQ1" s="2" t="s">
+      <c r="HO1" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="HR1" s="2" t="s">
+      <c r="HP1" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="HS1" s="2" t="s">
+      <c r="HQ1" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="HT1" s="2" t="s">
+      <c r="HR1" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="HU1" s="2" t="s">
+      <c r="HS1" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="HV1" s="2" t="s">
+      <c r="HT1" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="HW1" s="2" t="s">
+      <c r="HU1" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="HX1" s="2" t="s">
+      <c r="HV1" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="HY1" s="2" t="s">
+      <c r="HW1" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="HZ1" s="2" t="s">
+      <c r="HX1" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="IA1" s="2" t="s">
+      <c r="HY1" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="IB1" s="2" t="s">
+      <c r="HZ1" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="IC1" s="2" t="s">
+      <c r="IA1" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="ID1" s="2" t="s">
+      <c r="IB1" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="IE1" s="2" t="s">
+      <c r="IC1" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="IF1" s="2" t="s">
+      <c r="ID1" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="IG1" s="2" t="s">
+      <c r="IE1" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="IH1" s="2" t="s">
+      <c r="IF1" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="II1" s="2" t="s">
+      <c r="IG1" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="IJ1" s="2" t="s">
+      <c r="IH1" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="IK1" s="2" t="s">
+      <c r="II1" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="IL1" s="2" t="s">
+      <c r="IJ1" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="IM1" s="2" t="s">
+      <c r="IK1" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="IN1" s="2" t="s">
+      <c r="IL1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="IO1" s="2" t="s">
+      <c r="IM1" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="IP1" s="2" t="s">
+      <c r="IN1" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="IQ1" s="2" t="s">
+      <c r="IO1" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="IR1" s="2" t="s">
+      <c r="IP1" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="IS1" s="2" t="s">
+      <c r="IQ1" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="IT1" s="2" t="s">
+      <c r="IR1" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="IU1" s="2" t="s">
+      <c r="IS1" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="IV1" s="2" t="s">
+      <c r="IT1" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="IW1" s="2" t="s">
+      <c r="IU1" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="IX1" s="2" t="s">
+      <c r="IV1" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="IY1" s="2" t="s">
+      <c r="IW1" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="IZ1" s="2" t="s">
+      <c r="IX1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="JA1" s="2" t="s">
+      <c r="IY1" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="JB1" s="2" t="s">
+      <c r="IZ1" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="JC1" s="2" t="s">
+      <c r="JA1" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="JD1" s="2" t="s">
+      <c r="JB1" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="JE1" s="2" t="s">
+      <c r="JC1" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="JF1" s="2" t="s">
+      <c r="JD1" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="JG1" s="2" t="s">
+      <c r="JE1" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="JH1" s="2" t="s">
+      <c r="JF1" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="JI1" s="2" t="s">
+      <c r="JG1" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="JJ1" s="2" t="s">
+      <c r="JH1" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="JK1" s="2" t="s">
+      <c r="JI1" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="JL1" s="2" t="s">
+      <c r="JJ1" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="JM1" s="2" t="s">
+      <c r="JK1" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="JN1" s="2" t="s">
+      <c r="JL1" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="JO1" s="2" t="s">
+      <c r="JM1" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="JP1" s="2" t="s">
+      <c r="JN1" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="JQ1" s="2" t="s">
+      <c r="JO1" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="JR1" s="2" t="s">
+      <c r="JP1" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="JS1" s="2" t="s">
+      <c r="JQ1" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="JT1" s="2" t="s">
+      <c r="JR1" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="JU1" s="2" t="s">
+      <c r="JS1" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="JV1" s="2" t="s">
+      <c r="JT1" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="JW1" s="2" t="s">
+      <c r="JU1" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="JX1" s="2" t="s">
+      <c r="JV1" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="JY1" s="2" t="s">
+      <c r="JW1" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="JZ1" s="2" t="s">
+      <c r="JX1" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="KA1" s="2" t="s">
+      <c r="JY1" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="KB1" s="2" t="s">
+      <c r="JZ1" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="KC1" s="2" t="s">
+      <c r="KA1" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="KB1" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="KC1" s="7" t="s">
         <v>338</v>
       </c>
     </row>
@@ -2342,857 +2355,863 @@
       <c r="A2" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>287</v>
       </c>
+      <c r="C2" s="6">
+        <v>3.0019999999999998</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.9159999999999999</v>
+      </c>
       <c r="E2" s="6">
-        <v>3.0019999999999998</v>
+        <v>3.23</v>
       </c>
       <c r="F2" s="6">
-        <v>2.9159999999999999</v>
+        <v>3.4329999999999998</v>
       </c>
       <c r="G2" s="6">
-        <v>3.23</v>
+        <v>3.4809999999999999</v>
       </c>
       <c r="H2" s="6">
+        <v>3.605</v>
+      </c>
+      <c r="I2" s="6">
+        <v>4.024</v>
+      </c>
+      <c r="J2" s="6">
+        <v>4.09</v>
+      </c>
+      <c r="K2" s="6">
+        <v>3.504</v>
+      </c>
+      <c r="L2" s="6">
+        <v>3.47</v>
+      </c>
+      <c r="M2" s="6">
+        <v>3.1970000000000001</v>
+      </c>
+      <c r="N2" s="6">
+        <v>3.157</v>
+      </c>
+      <c r="O2" s="6">
+        <v>3.0649999999999999</v>
+      </c>
+      <c r="P2" s="6">
+        <v>2.9980000000000002</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>3.3809999999999998</v>
+      </c>
+      <c r="R2" s="6">
+        <v>3.4929999999999999</v>
+      </c>
+      <c r="S2" s="6">
+        <v>3.5979999999999999</v>
+      </c>
+      <c r="T2" s="6">
+        <v>3.6110000000000002</v>
+      </c>
+      <c r="U2" s="6">
+        <v>4.101</v>
+      </c>
+      <c r="V2" s="6">
+        <v>4.1959999999999997</v>
+      </c>
+      <c r="W2" s="6">
+        <v>3.5870000000000002</v>
+      </c>
+      <c r="X2" s="6">
+        <v>3.536</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>3.2189999999999999</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>3.2839999999999998</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>3.1070000000000002</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>3.0489999999999999</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>3.48</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>3.871</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>4.2270000000000003</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>4.3090000000000002</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>3.7440000000000002</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>3.6989999999999998</v>
+      </c>
+      <c r="AK2" s="6">
+        <v>3.323</v>
+      </c>
+      <c r="AL2" s="6">
+        <v>3.4460000000000002</v>
+      </c>
+      <c r="AM2" s="6">
+        <v>3.2469999999999999</v>
+      </c>
+      <c r="AN2" s="6">
+        <v>3.1890000000000001</v>
+      </c>
+      <c r="AO2" s="6">
+        <v>3.55</v>
+      </c>
+      <c r="AP2" s="6">
+        <v>3.7970000000000002</v>
+      </c>
+      <c r="AQ2" s="6">
+        <v>3.8780000000000001</v>
+      </c>
+      <c r="AR2" s="6">
+        <v>3.8980000000000001</v>
+      </c>
+      <c r="AS2" s="6">
+        <v>4.4009999999999998</v>
+      </c>
+      <c r="AT2" s="6">
+        <v>4.3789999999999996</v>
+      </c>
+      <c r="AU2" s="6">
+        <v>3.8380000000000001</v>
+      </c>
+      <c r="AV2" s="6">
+        <v>3.79</v>
+      </c>
+      <c r="AW2" s="6">
+        <v>3.4420000000000002</v>
+      </c>
+      <c r="AX2" s="6">
+        <v>3.5590000000000002</v>
+      </c>
+      <c r="AY2" s="6">
+        <v>3.375</v>
+      </c>
+      <c r="AZ2" s="6">
+        <v>3.206</v>
+      </c>
+      <c r="BA2" s="6">
+        <v>3.6859999999999999</v>
+      </c>
+      <c r="BB2" s="6">
+        <v>3.7509999999999999</v>
+      </c>
+      <c r="BC2" s="6">
+        <v>3.9470000000000001</v>
+      </c>
+      <c r="BD2" s="6">
+        <v>3.996</v>
+      </c>
+      <c r="BE2" s="6">
+        <v>4.4980000000000002</v>
+      </c>
+      <c r="BF2" s="6">
+        <v>4.4550000000000001</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>3.9239999999999999</v>
+      </c>
+      <c r="BH2" s="6">
+        <v>3.8580000000000001</v>
+      </c>
+      <c r="BI2" s="6">
+        <v>3.48</v>
+      </c>
+      <c r="BJ2" s="6">
+        <v>3.5659999999999998</v>
+      </c>
+      <c r="BK2" s="6">
+        <v>3.39</v>
+      </c>
+      <c r="BL2" s="6">
+        <v>3.2869999999999999</v>
+      </c>
+      <c r="BM2" s="6">
+        <v>3.6440000000000001</v>
+      </c>
+      <c r="BN2" s="6">
+        <v>3.8940000000000001</v>
+      </c>
+      <c r="BO2" s="6">
+        <v>3.9860000000000002</v>
+      </c>
+      <c r="BP2" s="6">
+        <v>4.0449999999999999</v>
+      </c>
+      <c r="BQ2" s="6">
+        <v>4.4980000000000002</v>
+      </c>
+      <c r="BR2" s="6">
+        <v>4.4560000000000004</v>
+      </c>
+      <c r="BS2" s="6">
+        <v>3.9849999999999999</v>
+      </c>
+      <c r="BT2" s="6">
+        <v>3.9340000000000002</v>
+      </c>
+      <c r="BU2" s="6">
+        <v>3.62</v>
+      </c>
+      <c r="BV2" s="6">
+        <v>3.6909999999999998</v>
+      </c>
+      <c r="BW2" s="6">
+        <v>3.484</v>
+      </c>
+      <c r="BX2" s="6">
+        <v>3.3639999999999999</v>
+      </c>
+      <c r="BY2" s="6">
+        <v>3.8050000000000002</v>
+      </c>
+      <c r="BZ2" s="6">
+        <v>3.9740000000000002</v>
+      </c>
+      <c r="CA2" s="6">
+        <v>3.956</v>
+      </c>
+      <c r="CB2" s="6">
+        <v>4.0880000000000001</v>
+      </c>
+      <c r="CC2" s="6">
+        <v>4.5410000000000004</v>
+      </c>
+      <c r="CD2" s="6">
+        <v>4.5519999999999996</v>
+      </c>
+      <c r="CE2" s="6">
+        <v>4.0519999999999996</v>
+      </c>
+      <c r="CF2" s="6">
+        <v>4.0090000000000003</v>
+      </c>
+      <c r="CG2" s="6">
+        <v>3.7080000000000002</v>
+      </c>
+      <c r="CH2" s="6">
+        <v>3.6629999999999998</v>
+      </c>
+      <c r="CI2" s="6">
+        <v>3.5569999999999999</v>
+      </c>
+      <c r="CJ2" s="6">
+        <v>3.4289999999999998</v>
+      </c>
+      <c r="CK2" s="6">
+        <v>3.7320000000000002</v>
+      </c>
+      <c r="CL2" s="6">
+        <v>3.895</v>
+      </c>
+      <c r="CM2" s="6">
+        <v>3.9940000000000002</v>
+      </c>
+      <c r="CN2" s="6">
+        <v>3.9550000000000001</v>
+      </c>
+      <c r="CO2" s="6">
+        <v>4.4450000000000003</v>
+      </c>
+      <c r="CP2" s="6">
+        <v>4.4930000000000003</v>
+      </c>
+      <c r="CQ2" s="6">
+        <v>3.9380000000000002</v>
+      </c>
+      <c r="CR2" s="6">
+        <v>3.9329999999999998</v>
+      </c>
+      <c r="CS2" s="6">
+        <v>3.528</v>
+      </c>
+      <c r="CT2" s="6">
+        <v>3.6309999999999998</v>
+      </c>
+      <c r="CU2" s="6">
+        <v>3.3969999999999998</v>
+      </c>
+      <c r="CV2" s="6">
+        <v>3.3420000000000001</v>
+      </c>
+      <c r="CW2" s="6">
+        <v>3.7080000000000002</v>
+      </c>
+      <c r="CX2" s="6">
+        <v>3.96</v>
+      </c>
+      <c r="CY2" s="6">
+        <v>4.0540000000000003</v>
+      </c>
+      <c r="CZ2" s="6">
+        <v>4.0629999999999997</v>
+      </c>
+      <c r="DA2" s="6">
+        <v>4.5289999999999999</v>
+      </c>
+      <c r="DB2" s="6">
+        <v>4.5890000000000004</v>
+      </c>
+      <c r="DC2" s="6">
+        <v>4.0410000000000004</v>
+      </c>
+      <c r="DD2" s="6">
+        <v>4.0629999999999997</v>
+      </c>
+      <c r="DE2" s="6">
+        <v>3.625</v>
+      </c>
+      <c r="DF2" s="6">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="DG2" s="6">
+        <v>3.4319999999999999</v>
+      </c>
+      <c r="DH2" s="6">
+        <v>3.4049999999999998</v>
+      </c>
+      <c r="DI2" s="6">
+        <v>3.819</v>
+      </c>
+      <c r="DJ2" s="6">
+        <v>4.1369999999999996</v>
+      </c>
+      <c r="DK2" s="6">
+        <v>4.17</v>
+      </c>
+      <c r="DL2" s="6">
+        <v>4.194</v>
+      </c>
+      <c r="DM2" s="6">
+        <v>4.665</v>
+      </c>
+      <c r="DN2" s="6">
+        <v>4.6470000000000002</v>
+      </c>
+      <c r="DO2" s="6">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="DP2" s="6">
+        <v>4.0860000000000003</v>
+      </c>
+      <c r="DQ2" s="6">
+        <v>3.7250000000000001</v>
+      </c>
+      <c r="DR2" s="6">
+        <v>3.6379999999999999</v>
+      </c>
+      <c r="DS2" s="6">
+        <v>3.6589999999999998</v>
+      </c>
+      <c r="DT2" s="6">
+        <v>3.5230000000000001</v>
+      </c>
+      <c r="DU2" s="6">
+        <v>3.9460000000000002</v>
+      </c>
+      <c r="DV2" s="6">
+        <v>4.1669999999999998</v>
+      </c>
+      <c r="DW2" s="6">
+        <v>4.2050000000000001</v>
+      </c>
+      <c r="DX2" s="6">
+        <v>4.3109999999999999</v>
+      </c>
+      <c r="DY2" s="6">
+        <v>4.7050000000000001</v>
+      </c>
+      <c r="DZ2" s="6">
+        <v>4.6890000000000001</v>
+      </c>
+      <c r="EA2" s="6">
+        <v>4.2119999999999997</v>
+      </c>
+      <c r="EB2" s="6">
+        <v>4.1890000000000001</v>
+      </c>
+      <c r="EC2" s="6">
+        <v>3.7749999999999999</v>
+      </c>
+      <c r="ED2" s="6">
+        <v>3.8769999999999998</v>
+      </c>
+      <c r="EE2" s="6">
+        <v>3.6909999999999998</v>
+      </c>
+      <c r="EF2" s="6">
+        <v>3.3860000000000001</v>
+      </c>
+      <c r="EG2" s="6">
+        <v>3.9430000000000001</v>
+      </c>
+      <c r="EH2" s="6">
+        <v>4.0259999999999998</v>
+      </c>
+      <c r="EI2" s="6">
+        <v>4.1680000000000001</v>
+      </c>
+      <c r="EJ2" s="6">
+        <v>4.2549999999999999</v>
+      </c>
+      <c r="EK2" s="6">
+        <v>4.681</v>
+      </c>
+      <c r="EL2" s="6">
+        <v>4.6769999999999996</v>
+      </c>
+      <c r="EM2" s="6">
+        <v>4.1959999999999997</v>
+      </c>
+      <c r="EN2" s="6">
+        <v>4.1289999999999996</v>
+      </c>
+      <c r="EO2" s="6">
+        <v>3.835</v>
+      </c>
+      <c r="EP2" s="6">
+        <v>3.7480000000000002</v>
+      </c>
+      <c r="EQ2" s="6">
+        <v>3.593</v>
+      </c>
+      <c r="ER2" s="6">
         <v>3.4329999999999998</v>
       </c>
-      <c r="I2" s="6">
-        <v>3.4809999999999999</v>
-      </c>
-      <c r="J2" s="6">
-        <v>3.605</v>
-      </c>
-      <c r="K2" s="6">
-        <v>4.024</v>
-      </c>
-      <c r="L2" s="6">
-        <v>4.09</v>
-      </c>
-      <c r="M2" s="6">
-        <v>3.504</v>
-      </c>
-      <c r="N2" s="6">
-        <v>3.47</v>
-      </c>
-      <c r="O2" s="6">
-        <v>3.1970000000000001</v>
-      </c>
-      <c r="P2" s="6">
-        <v>3.157</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>3.0649999999999999</v>
-      </c>
-      <c r="R2" s="6">
-        <v>2.9980000000000002</v>
-      </c>
-      <c r="S2" s="6">
-        <v>3.3809999999999998</v>
-      </c>
-      <c r="T2" s="6">
-        <v>3.4929999999999999</v>
-      </c>
-      <c r="U2" s="6">
-        <v>3.5979999999999999</v>
-      </c>
-      <c r="V2" s="6">
-        <v>3.6110000000000002</v>
-      </c>
-      <c r="W2" s="6">
-        <v>4.101</v>
-      </c>
-      <c r="X2" s="6">
-        <v>4.1959999999999997</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>3.5870000000000002</v>
-      </c>
-      <c r="Z2" s="6">
-        <v>3.536</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>3.2189999999999999</v>
-      </c>
-      <c r="AB2" s="6">
-        <v>3.2839999999999998</v>
-      </c>
-      <c r="AC2" s="6">
-        <v>3.1070000000000002</v>
-      </c>
-      <c r="AD2" s="6">
-        <v>3.0489999999999999</v>
-      </c>
-      <c r="AE2" s="6">
-        <v>3.48</v>
-      </c>
-      <c r="AF2" s="6">
-        <v>3.6720000000000002</v>
-      </c>
-      <c r="AG2" s="6">
-        <v>3.6589999999999998</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>3.871</v>
-      </c>
-      <c r="AI2" s="6">
+      <c r="ES2" s="6">
+        <v>3.9180000000000001</v>
+      </c>
+      <c r="ET2" s="6">
+        <v>4.04</v>
+      </c>
+      <c r="EU2" s="6">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="EV2" s="6">
+        <v>4.2629999999999999</v>
+      </c>
+      <c r="EW2" s="6">
+        <v>4.7389999999999999</v>
+      </c>
+      <c r="EX2" s="6">
+        <v>4.7539999999999996</v>
+      </c>
+      <c r="EY2" s="6">
+        <v>4.22</v>
+      </c>
+      <c r="EZ2" s="6">
+        <v>4.2510000000000003</v>
+      </c>
+      <c r="FA2" s="6">
+        <v>3.7930000000000001</v>
+      </c>
+      <c r="FB2" s="6">
+        <v>3.867</v>
+      </c>
+      <c r="FC2" s="6">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="FD2" s="6">
+        <v>3.4689999999999999</v>
+      </c>
+      <c r="FE2" s="6">
+        <v>3.9319999999999999</v>
+      </c>
+      <c r="FF2" s="6">
+        <v>4.0919999999999996</v>
+      </c>
+      <c r="FG2" s="6">
+        <v>4.1429999999999998</v>
+      </c>
+      <c r="FH2" s="6">
+        <v>4.3390000000000004</v>
+      </c>
+      <c r="FI2" s="6">
+        <v>4.665</v>
+      </c>
+      <c r="FJ2" s="6">
+        <v>4.7279999999999998</v>
+      </c>
+      <c r="FK2" s="6">
+        <v>4.202</v>
+      </c>
+      <c r="FL2" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="FM2" s="6">
+        <v>3.7610000000000001</v>
+      </c>
+      <c r="FN2" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="FO2" s="6">
+        <v>3.6840000000000002</v>
+      </c>
+      <c r="FP2" s="6">
+        <v>3.5339999999999998</v>
+      </c>
+      <c r="FQ2" s="6">
+        <v>3.9449999999999998</v>
+      </c>
+      <c r="FR2" s="6">
+        <v>4.1859999999999999</v>
+      </c>
+      <c r="FS2" s="6">
+        <v>4.26</v>
+      </c>
+      <c r="FT2" s="6">
+        <v>4.3890000000000002</v>
+      </c>
+      <c r="FU2" s="6">
+        <v>4.7679999999999998</v>
+      </c>
+      <c r="FV2" s="6">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="FW2" s="6">
+        <v>4.2610000000000001</v>
+      </c>
+      <c r="FX2" s="6">
+        <v>4.3289999999999997</v>
+      </c>
+      <c r="FY2" s="6">
+        <v>3.7970000000000002</v>
+      </c>
+      <c r="FZ2" s="6">
+        <v>4.0330000000000004</v>
+      </c>
+      <c r="GA2" s="6">
+        <v>3.6579999999999999</v>
+      </c>
+      <c r="GB2" s="6">
+        <v>3.5419999999999998</v>
+      </c>
+      <c r="GC2" s="6">
+        <v>3.9670000000000001</v>
+      </c>
+      <c r="GD2" s="6">
+        <v>4.0880000000000001</v>
+      </c>
+      <c r="GE2" s="6">
+        <v>4.181</v>
+      </c>
+      <c r="GF2" s="6">
+        <v>4.3230000000000004</v>
+      </c>
+      <c r="GG2" s="6">
+        <v>4.8230000000000004</v>
+      </c>
+      <c r="GH2" s="6">
+        <v>4.71</v>
+      </c>
+      <c r="GI2" s="6">
+        <v>4.2229999999999999</v>
+      </c>
+      <c r="GJ2" s="6">
+        <v>4.2640000000000002</v>
+      </c>
+      <c r="GK2" s="6">
+        <v>3.8090000000000002</v>
+      </c>
+      <c r="GL2" s="6">
+        <v>3.9929999999999999</v>
+      </c>
+      <c r="GM2" s="6">
+        <v>3.774</v>
+      </c>
+      <c r="GN2" s="6">
+        <v>3.73</v>
+      </c>
+      <c r="GO2" s="6">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="GP2" s="6">
+        <v>4.3159999999999998</v>
+      </c>
+      <c r="GQ2" s="6">
+        <v>4.391</v>
+      </c>
+      <c r="GR2" s="6">
+        <v>4.5410000000000004</v>
+      </c>
+      <c r="GS2" s="6">
+        <v>4.9080000000000004</v>
+      </c>
+      <c r="GT2" s="6">
+        <v>4.8360000000000003</v>
+      </c>
+      <c r="GU2" s="6">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="GV2" s="6">
+        <v>4.4249999999999998</v>
+      </c>
+      <c r="GW2" s="6">
+        <v>3.984</v>
+      </c>
+      <c r="GX2" s="6">
+        <v>4.0309999999999997</v>
+      </c>
+      <c r="GY2" s="6">
+        <v>3.8839999999999999</v>
+      </c>
+      <c r="GZ2" s="6">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="HA2" s="6">
+        <v>4.1159999999999997</v>
+      </c>
+      <c r="HB2" s="6">
         <v>4.2270000000000003</v>
       </c>
-      <c r="AJ2" s="6">
-        <v>4.3090000000000002</v>
-      </c>
-      <c r="AK2" s="6">
-        <v>3.7440000000000002</v>
-      </c>
-      <c r="AL2" s="6">
+      <c r="HC2" s="6">
+        <v>4.3760000000000003</v>
+      </c>
+      <c r="HD2" s="6">
+        <v>4.4550000000000001</v>
+      </c>
+      <c r="HE2" s="6">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="HF2" s="6">
+        <v>4.8019999999999996</v>
+      </c>
+      <c r="HG2" s="6">
+        <v>4.2839999999999998</v>
+      </c>
+      <c r="HH2" s="6">
+        <v>4.4089999999999998</v>
+      </c>
+      <c r="HI2" s="6">
+        <v>3.7869999999999999</v>
+      </c>
+      <c r="HJ2" s="6">
+        <v>3.8660000000000001</v>
+      </c>
+      <c r="HK2" s="6">
+        <v>3.8170000000000002</v>
+      </c>
+      <c r="HL2" s="6">
+        <v>3.714</v>
+      </c>
+      <c r="HM2" s="6">
+        <v>4.1130000000000004</v>
+      </c>
+      <c r="HN2" s="6">
+        <v>4.335</v>
+      </c>
+      <c r="HO2" s="6">
+        <v>4.2930000000000001</v>
+      </c>
+      <c r="HP2" s="6">
+        <v>4.5490000000000004</v>
+      </c>
+      <c r="HQ2" s="6">
+        <v>4.8760000000000003</v>
+      </c>
+      <c r="HR2" s="6">
+        <v>4.8780000000000001</v>
+      </c>
+      <c r="HS2" s="6">
+        <v>4.3390000000000004</v>
+      </c>
+      <c r="HT2" s="6">
+        <v>4.4180000000000001</v>
+      </c>
+      <c r="HU2" s="6">
+        <v>3.9670000000000001</v>
+      </c>
+      <c r="HV2" s="6">
+        <v>4.1020000000000003</v>
+      </c>
+      <c r="HW2" s="6">
+        <v>3.84</v>
+      </c>
+      <c r="HX2" s="6">
+        <v>3.6509999999999998</v>
+      </c>
+      <c r="HY2" s="6">
+        <v>2.4380000000000002</v>
+      </c>
+      <c r="HZ2" s="6">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="IA2" s="6">
+        <v>2.4729999999999999</v>
+      </c>
+      <c r="IB2" s="6">
+        <v>3.9940000000000002</v>
+      </c>
+      <c r="IC2" s="6">
+        <v>4.7229999999999999</v>
+      </c>
+      <c r="ID2" s="6">
+        <v>4.6859999999999999</v>
+      </c>
+      <c r="IE2" s="6">
+        <v>4.1020000000000003</v>
+      </c>
+      <c r="IF2" s="6">
+        <v>4.0720000000000001</v>
+      </c>
+      <c r="IG2" s="6">
+        <v>2.4969999999999999</v>
+      </c>
+      <c r="IH2" s="6">
+        <v>3.37</v>
+      </c>
+      <c r="II2" s="6">
+        <v>3.4049999999999998</v>
+      </c>
+      <c r="IJ2" s="6">
+        <v>3.3319999999999999</v>
+      </c>
+      <c r="IK2" s="6">
+        <v>3.6539999999999999</v>
+      </c>
+      <c r="IL2" s="6">
+        <v>3.044</v>
+      </c>
+      <c r="IM2" s="6">
+        <v>3.8820000000000001</v>
+      </c>
+      <c r="IN2" s="6">
+        <v>4.3550000000000004</v>
+      </c>
+      <c r="IO2" s="6">
+        <v>4.931</v>
+      </c>
+      <c r="IP2" s="6">
+        <v>4.8490000000000002</v>
+      </c>
+      <c r="IQ2" s="6">
+        <v>4.3849999999999998</v>
+      </c>
+      <c r="IR2" s="6">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="IS2" s="6">
+        <v>3.927</v>
+      </c>
+      <c r="IT2" s="6">
+        <v>3.9710000000000001</v>
+      </c>
+      <c r="IU2" s="6">
         <v>3.6989999999999998</v>
       </c>
-      <c r="AM2" s="6">
-        <v>3.323</v>
-      </c>
-      <c r="AN2" s="6">
-        <v>3.4460000000000002</v>
-      </c>
-      <c r="AO2" s="6">
-        <v>3.2469999999999999</v>
-      </c>
-      <c r="AP2" s="6">
-        <v>3.1890000000000001</v>
-      </c>
-      <c r="AQ2" s="6">
-        <v>3.55</v>
-      </c>
-      <c r="AR2" s="6">
-        <v>3.7970000000000002</v>
-      </c>
-      <c r="AS2" s="6">
-        <v>3.8780000000000001</v>
-      </c>
-      <c r="AT2" s="6">
-        <v>3.8980000000000001</v>
-      </c>
-      <c r="AU2" s="6">
-        <v>4.4009999999999998</v>
-      </c>
-      <c r="AV2" s="6">
-        <v>4.3789999999999996</v>
-      </c>
-      <c r="AW2" s="6">
-        <v>3.8380000000000001</v>
-      </c>
-      <c r="AX2" s="6">
-        <v>3.79</v>
-      </c>
-      <c r="AY2" s="6">
-        <v>3.4420000000000002</v>
-      </c>
-      <c r="AZ2" s="6">
-        <v>3.5590000000000002</v>
-      </c>
-      <c r="BA2" s="6">
-        <v>3.375</v>
-      </c>
-      <c r="BB2" s="6">
-        <v>3.206</v>
-      </c>
-      <c r="BC2" s="6">
-        <v>3.6859999999999999</v>
-      </c>
-      <c r="BD2" s="6">
-        <v>3.7509999999999999</v>
-      </c>
-      <c r="BE2" s="6">
-        <v>3.9470000000000001</v>
-      </c>
-      <c r="BF2" s="6">
-        <v>3.996</v>
-      </c>
-      <c r="BG2" s="6">
-        <v>4.4980000000000002</v>
-      </c>
-      <c r="BH2" s="6">
-        <v>4.4550000000000001</v>
-      </c>
-      <c r="BI2" s="6">
-        <v>3.9239999999999999</v>
-      </c>
-      <c r="BJ2" s="6">
-        <v>3.8580000000000001</v>
-      </c>
-      <c r="BK2" s="6">
-        <v>3.48</v>
-      </c>
-      <c r="BL2" s="6">
-        <v>3.5659999999999998</v>
-      </c>
-      <c r="BM2" s="6">
-        <v>3.39</v>
-      </c>
-      <c r="BN2" s="6">
-        <v>3.2869999999999999</v>
-      </c>
-      <c r="BO2" s="6">
-        <v>3.6440000000000001</v>
-      </c>
-      <c r="BP2" s="6">
-        <v>3.8940000000000001</v>
-      </c>
-      <c r="BQ2" s="6">
-        <v>3.9860000000000002</v>
-      </c>
-      <c r="BR2" s="6">
-        <v>4.0449999999999999</v>
-      </c>
-      <c r="BS2" s="6">
-        <v>4.4980000000000002</v>
-      </c>
-      <c r="BT2" s="6">
-        <v>4.4560000000000004</v>
-      </c>
-      <c r="BU2" s="6">
-        <v>3.9849999999999999</v>
-      </c>
-      <c r="BV2" s="6">
-        <v>3.9340000000000002</v>
-      </c>
-      <c r="BW2" s="6">
-        <v>3.62</v>
-      </c>
-      <c r="BX2" s="6">
-        <v>3.6909999999999998</v>
-      </c>
-      <c r="BY2" s="6">
-        <v>3.484</v>
-      </c>
-      <c r="BZ2" s="6">
-        <v>3.3639999999999999</v>
-      </c>
-      <c r="CA2" s="6">
-        <v>3.8050000000000002</v>
-      </c>
-      <c r="CB2" s="6">
-        <v>3.9740000000000002</v>
-      </c>
-      <c r="CC2" s="6">
-        <v>3.956</v>
-      </c>
-      <c r="CD2" s="6">
-        <v>4.0880000000000001</v>
-      </c>
-      <c r="CE2" s="6">
-        <v>4.5410000000000004</v>
-      </c>
-      <c r="CF2" s="6">
-        <v>4.5519999999999996</v>
-      </c>
-      <c r="CG2" s="6">
-        <v>4.0519999999999996</v>
-      </c>
-      <c r="CH2" s="6">
-        <v>4.0090000000000003</v>
-      </c>
-      <c r="CI2" s="6">
+      <c r="IV2" s="6">
+        <v>3.74</v>
+      </c>
+      <c r="IW2" s="6">
+        <v>3.9430000000000001</v>
+      </c>
+      <c r="IX2" s="6">
+        <v>3.98</v>
+      </c>
+      <c r="IY2" s="6">
+        <v>4.375</v>
+      </c>
+      <c r="IZ2" s="6">
+        <v>4.5110000000000001</v>
+      </c>
+      <c r="JA2" s="6">
+        <v>4.8360000000000003</v>
+      </c>
+      <c r="JB2" s="6">
+        <v>4.7949999999999999</v>
+      </c>
+      <c r="JC2" s="6">
+        <v>4.2990000000000004</v>
+      </c>
+      <c r="JD2" s="6">
+        <v>4.2130000000000001</v>
+      </c>
+      <c r="JE2" s="6">
+        <v>3.923</v>
+      </c>
+      <c r="JF2" s="6">
+        <v>3.8719999999999999</v>
+      </c>
+      <c r="JG2" s="6">
+        <v>3.7879999999999998</v>
+      </c>
+      <c r="JH2" s="6">
+        <v>3.758</v>
+      </c>
+      <c r="JI2" s="6">
+        <v>3.9079999999999999</v>
+      </c>
+      <c r="JJ2" s="6">
+        <v>4.0259999999999998</v>
+      </c>
+      <c r="JK2" s="6">
+        <v>4.3579999999999997</v>
+      </c>
+      <c r="JL2" s="6">
+        <v>4.5759999999999996</v>
+      </c>
+      <c r="JM2" s="6">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="JN2" s="6">
+        <v>4.7880000000000003</v>
+      </c>
+      <c r="JO2" s="6">
+        <v>4.3220000000000001</v>
+      </c>
+      <c r="JP2" s="6">
+        <v>4.3410000000000002</v>
+      </c>
+      <c r="JQ2" s="6">
+        <v>3.8740000000000001</v>
+      </c>
+      <c r="JR2" s="6">
+        <v>3.9220000000000002</v>
+      </c>
+      <c r="JS2" s="6">
+        <v>3.7770000000000001</v>
+      </c>
+      <c r="JT2" s="6">
         <v>3.7080000000000002</v>
       </c>
-      <c r="CJ2" s="6">
-        <v>3.6629999999999998</v>
-      </c>
-      <c r="CK2" s="6">
-        <v>3.5569999999999999</v>
-      </c>
-      <c r="CL2" s="6">
-        <v>3.4289999999999998</v>
-      </c>
-      <c r="CM2" s="6">
-        <v>3.7320000000000002</v>
-      </c>
-      <c r="CN2" s="6">
-        <v>3.895</v>
-      </c>
-      <c r="CO2" s="6">
-        <v>3.9940000000000002</v>
-      </c>
-      <c r="CP2" s="6">
-        <v>3.9550000000000001</v>
-      </c>
-      <c r="CQ2" s="6">
+      <c r="JU2" s="6">
+        <v>4.0119999999999996</v>
+      </c>
+      <c r="JV2" s="6">
+        <v>3.97</v>
+      </c>
+      <c r="JW2" s="6">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="JX2" s="6">
         <v>4.4450000000000003</v>
       </c>
-      <c r="CR2" s="6">
-        <v>4.4930000000000003</v>
-      </c>
-      <c r="CS2" s="6">
-        <v>3.9380000000000002</v>
-      </c>
-      <c r="CT2" s="6">
-        <v>3.9329999999999998</v>
-      </c>
-      <c r="CU2" s="6">
-        <v>3.528</v>
-      </c>
-      <c r="CV2" s="6">
-        <v>3.6309999999999998</v>
-      </c>
-      <c r="CW2" s="6">
-        <v>3.3969999999999998</v>
-      </c>
-      <c r="CX2" s="6">
-        <v>3.3420000000000001</v>
-      </c>
-      <c r="CY2" s="6">
-        <v>3.7080000000000002</v>
-      </c>
-      <c r="CZ2" s="6">
-        <v>3.96</v>
-      </c>
-      <c r="DA2" s="6">
-        <v>4.0540000000000003</v>
-      </c>
-      <c r="DB2" s="6">
-        <v>4.0629999999999997</v>
-      </c>
-      <c r="DC2" s="6">
-        <v>4.5289999999999999</v>
-      </c>
-      <c r="DD2" s="6">
-        <v>4.5890000000000004</v>
-      </c>
-      <c r="DE2" s="6">
-        <v>4.0410000000000004</v>
-      </c>
-      <c r="DF2" s="6">
-        <v>4.0629999999999997</v>
-      </c>
-      <c r="DG2" s="6">
-        <v>3.625</v>
-      </c>
-      <c r="DH2" s="6">
-        <v>3.6259999999999999</v>
-      </c>
-      <c r="DI2" s="6">
-        <v>3.4319999999999999</v>
-      </c>
-      <c r="DJ2" s="6">
-        <v>3.4049999999999998</v>
-      </c>
-      <c r="DK2" s="6">
-        <v>3.819</v>
-      </c>
-      <c r="DL2" s="6">
-        <v>4.1369999999999996</v>
-      </c>
-      <c r="DM2" s="6">
-        <v>4.17</v>
-      </c>
-      <c r="DN2" s="6">
-        <v>4.194</v>
-      </c>
-      <c r="DO2" s="6">
-        <v>4.665</v>
-      </c>
-      <c r="DP2" s="6">
-        <v>4.6470000000000002</v>
-      </c>
-      <c r="DQ2" s="6">
-        <v>4.1399999999999997</v>
-      </c>
-      <c r="DR2" s="6">
-        <v>4.0860000000000003</v>
-      </c>
-      <c r="DS2" s="6">
-        <v>3.7250000000000001</v>
-      </c>
-      <c r="DT2" s="6">
-        <v>3.6379999999999999</v>
-      </c>
-      <c r="DU2" s="6">
-        <v>3.6589999999999998</v>
-      </c>
-      <c r="DV2" s="6">
-        <v>3.5230000000000001</v>
-      </c>
-      <c r="DW2" s="6">
-        <v>3.9460000000000002</v>
-      </c>
-      <c r="DX2" s="6">
-        <v>4.1669999999999998</v>
-      </c>
-      <c r="DY2" s="6">
-        <v>4.2050000000000001</v>
-      </c>
-      <c r="DZ2" s="6">
-        <v>4.3109999999999999</v>
-      </c>
-      <c r="EA2" s="6">
-        <v>4.7050000000000001</v>
-      </c>
-      <c r="EB2" s="6">
-        <v>4.6890000000000001</v>
-      </c>
-      <c r="EC2" s="6">
-        <v>4.2119999999999997</v>
-      </c>
-      <c r="ED2" s="6">
-        <v>4.1890000000000001</v>
-      </c>
-      <c r="EE2" s="6">
-        <v>3.7749999999999999</v>
-      </c>
-      <c r="EF2" s="6">
-        <v>3.8769999999999998</v>
-      </c>
-      <c r="EG2" s="6">
-        <v>3.6909999999999998</v>
-      </c>
-      <c r="EH2" s="6">
-        <v>3.3860000000000001</v>
-      </c>
-      <c r="EI2" s="6">
-        <v>3.9430000000000001</v>
-      </c>
-      <c r="EJ2" s="6">
-        <v>4.0259999999999998</v>
-      </c>
-      <c r="EK2" s="6">
-        <v>4.1680000000000001</v>
-      </c>
-      <c r="EL2" s="6">
-        <v>4.2549999999999999</v>
-      </c>
-      <c r="EM2" s="6">
-        <v>4.681</v>
-      </c>
-      <c r="EN2" s="6">
-        <v>4.6769999999999996</v>
-      </c>
-      <c r="EO2" s="6">
-        <v>4.1959999999999997</v>
-      </c>
-      <c r="EP2" s="6">
-        <v>4.1289999999999996</v>
-      </c>
-      <c r="EQ2" s="6">
-        <v>3.835</v>
-      </c>
-      <c r="ER2" s="6">
-        <v>3.7480000000000002</v>
-      </c>
-      <c r="ES2" s="6">
-        <v>3.593</v>
-      </c>
-      <c r="ET2" s="6">
-        <v>3.4329999999999998</v>
-      </c>
-      <c r="EU2" s="6">
-        <v>3.9180000000000001</v>
-      </c>
-      <c r="EV2" s="6">
-        <v>4.04</v>
-      </c>
-      <c r="EW2" s="6">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="EX2" s="6">
-        <v>4.2629999999999999</v>
-      </c>
-      <c r="EY2" s="6">
-        <v>4.7389999999999999</v>
-      </c>
-      <c r="EZ2" s="6">
-        <v>4.7539999999999996</v>
-      </c>
-      <c r="FA2" s="6">
-        <v>4.22</v>
-      </c>
-      <c r="FB2" s="6">
-        <v>4.2510000000000003</v>
-      </c>
-      <c r="FC2" s="6">
-        <v>3.7930000000000001</v>
-      </c>
-      <c r="FD2" s="6">
-        <v>3.867</v>
-      </c>
-      <c r="FE2" s="6">
-        <v>3.6960000000000002</v>
-      </c>
-      <c r="FF2" s="6">
-        <v>3.4689999999999999</v>
-      </c>
-      <c r="FG2" s="6">
-        <v>3.9319999999999999</v>
-      </c>
-      <c r="FH2" s="6">
-        <v>4.0919999999999996</v>
-      </c>
-      <c r="FI2" s="6">
-        <v>4.1429999999999998</v>
-      </c>
-      <c r="FJ2" s="6">
-        <v>4.3390000000000004</v>
-      </c>
-      <c r="FK2" s="6">
-        <v>4.665</v>
-      </c>
-      <c r="FL2" s="6">
-        <v>4.7279999999999998</v>
-      </c>
-      <c r="FM2" s="6">
-        <v>4.202</v>
-      </c>
-      <c r="FN2" s="6">
-        <v>4.3</v>
-      </c>
-      <c r="FO2" s="6">
-        <v>3.7610000000000001</v>
-      </c>
-      <c r="FP2" s="6">
-        <v>3.9</v>
-      </c>
-      <c r="FQ2" s="6">
-        <v>3.6840000000000002</v>
-      </c>
-      <c r="FR2" s="6">
-        <v>3.5339999999999998</v>
-      </c>
-      <c r="FS2" s="6">
-        <v>3.9449999999999998</v>
-      </c>
-      <c r="FT2" s="6">
-        <v>4.1859999999999999</v>
-      </c>
-      <c r="FU2" s="6">
-        <v>4.26</v>
-      </c>
-      <c r="FV2" s="6">
-        <v>4.3890000000000002</v>
-      </c>
-      <c r="FW2" s="6">
-        <v>4.7679999999999998</v>
-      </c>
-      <c r="FX2" s="6">
-        <v>4.7830000000000004</v>
-      </c>
-      <c r="FY2" s="6">
-        <v>4.2610000000000001</v>
-      </c>
-      <c r="FZ2" s="6">
-        <v>4.3289999999999997</v>
-      </c>
-      <c r="GA2" s="6">
-        <v>3.7970000000000002</v>
-      </c>
-      <c r="GB2" s="6">
-        <v>4.0330000000000004</v>
-      </c>
-      <c r="GC2" s="6">
-        <v>3.6579999999999999</v>
-      </c>
-      <c r="GD2" s="6">
-        <v>3.5419999999999998</v>
-      </c>
-      <c r="GE2" s="6">
-        <v>3.9670000000000001</v>
-      </c>
-      <c r="GF2" s="6">
-        <v>4.0880000000000001</v>
-      </c>
-      <c r="GG2" s="6">
-        <v>4.181</v>
-      </c>
-      <c r="GH2" s="6">
-        <v>4.3230000000000004</v>
-      </c>
-      <c r="GI2" s="6">
+      <c r="JY2" s="6">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="JZ2" s="6">
         <v>4.8230000000000004</v>
       </c>
-      <c r="GJ2" s="6">
-        <v>4.71</v>
-      </c>
-      <c r="GK2" s="6">
-        <v>4.2229999999999999</v>
-      </c>
-      <c r="GL2" s="6">
-        <v>4.2640000000000002</v>
-      </c>
-      <c r="GM2" s="6">
-        <v>3.8090000000000002</v>
-      </c>
-      <c r="GN2" s="6">
-        <v>3.9929999999999999</v>
-      </c>
-      <c r="GO2" s="6">
-        <v>3.774</v>
-      </c>
-      <c r="GP2" s="6">
-        <v>3.73</v>
-      </c>
-      <c r="GQ2" s="6">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="GR2" s="6">
-        <v>4.3159999999999998</v>
-      </c>
-      <c r="GS2" s="6">
-        <v>4.391</v>
-      </c>
-      <c r="GT2" s="6">
-        <v>4.5410000000000004</v>
-      </c>
-      <c r="GU2" s="6">
-        <v>4.9080000000000004</v>
-      </c>
-      <c r="GV2" s="6">
-        <v>4.8360000000000003</v>
-      </c>
-      <c r="GW2" s="6">
-        <v>4.3479999999999999</v>
-      </c>
-      <c r="GX2" s="6">
-        <v>4.4249999999999998</v>
-      </c>
-      <c r="GY2" s="6">
-        <v>3.984</v>
-      </c>
-      <c r="GZ2" s="6">
-        <v>4.0309999999999997</v>
-      </c>
-      <c r="HA2" s="6">
-        <v>3.8839999999999999</v>
-      </c>
-      <c r="HB2" s="6">
-        <v>3.6259999999999999</v>
-      </c>
-      <c r="HC2" s="6">
-        <v>4.1159999999999997</v>
-      </c>
-      <c r="HD2" s="6">
-        <v>4.2270000000000003</v>
-      </c>
-      <c r="HE2" s="6">
-        <v>4.3760000000000003</v>
-      </c>
-      <c r="HF2" s="6">
-        <v>4.4550000000000001</v>
-      </c>
-      <c r="HG2" s="6">
-        <v>4.8070000000000004</v>
-      </c>
-      <c r="HH2" s="6">
-        <v>4.8019999999999996</v>
-      </c>
-      <c r="HI2" s="6">
-        <v>4.2839999999999998</v>
-      </c>
-      <c r="HJ2" s="6">
-        <v>4.4089999999999998</v>
-      </c>
-      <c r="HK2" s="6">
-        <v>3.7869999999999999</v>
-      </c>
-      <c r="HL2" s="6">
-        <v>3.8660000000000001</v>
-      </c>
-      <c r="HM2" s="6">
-        <v>3.8170000000000002</v>
-      </c>
-      <c r="HN2" s="6">
-        <v>3.714</v>
-      </c>
-      <c r="HO2" s="6">
-        <v>4.1130000000000004</v>
-      </c>
-      <c r="HP2" s="6">
-        <v>4.335</v>
-      </c>
-      <c r="HQ2" s="6">
-        <v>4.2930000000000001</v>
-      </c>
-      <c r="HR2" s="6">
-        <v>4.5490000000000004</v>
-      </c>
-      <c r="HS2" s="6">
-        <v>4.8760000000000003</v>
-      </c>
-      <c r="HT2" s="6">
-        <v>4.8780000000000001</v>
-      </c>
-      <c r="HU2" s="6">
-        <v>4.3390000000000004</v>
-      </c>
-      <c r="HV2" s="6">
-        <v>4.4180000000000001</v>
-      </c>
-      <c r="HW2" s="6">
-        <v>3.9670000000000001</v>
-      </c>
-      <c r="HX2" s="6">
-        <v>4.1020000000000003</v>
-      </c>
-      <c r="HY2" s="6">
-        <v>3.84</v>
-      </c>
-      <c r="HZ2" s="6">
-        <v>3.6509999999999998</v>
-      </c>
-      <c r="IA2" s="6">
-        <v>2.4380000000000002</v>
-      </c>
-      <c r="IB2" s="6">
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="IC2" s="6">
-        <v>2.4729999999999999</v>
-      </c>
-      <c r="ID2" s="6">
-        <v>3.9940000000000002</v>
-      </c>
-      <c r="IE2" s="6">
-        <v>4.7229999999999999</v>
-      </c>
-      <c r="IF2" s="6">
-        <v>4.6859999999999999</v>
-      </c>
-      <c r="IG2" s="6">
-        <v>4.1020000000000003</v>
-      </c>
-      <c r="IH2" s="6">
-        <v>4.0720000000000001</v>
-      </c>
-      <c r="II2" s="6">
-        <v>2.4969999999999999</v>
-      </c>
-      <c r="IJ2" s="6">
-        <v>3.37</v>
-      </c>
-      <c r="IK2" s="6">
-        <v>3.4049999999999998</v>
-      </c>
-      <c r="IL2" s="6">
-        <v>3.3319999999999999</v>
-      </c>
-      <c r="IM2" s="6">
-        <v>3.6539999999999999</v>
-      </c>
-      <c r="IN2" s="6">
-        <v>3.044</v>
-      </c>
-      <c r="IO2" s="6">
-        <v>3.8820000000000001</v>
-      </c>
-      <c r="IP2" s="6">
-        <v>4.3550000000000004</v>
-      </c>
-      <c r="IQ2" s="6">
-        <v>4.931</v>
-      </c>
-      <c r="IR2" s="6">
-        <v>4.8490000000000002</v>
-      </c>
-      <c r="IS2" s="6">
-        <v>4.3849999999999998</v>
-      </c>
-      <c r="IT2" s="6">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="IU2" s="6">
-        <v>3.927</v>
-      </c>
-      <c r="IV2" s="6">
-        <v>3.9710000000000001</v>
-      </c>
-      <c r="IW2" s="6">
-        <v>3.6989999999999998</v>
-      </c>
-      <c r="IX2" s="6">
-        <v>3.74</v>
-      </c>
-      <c r="IY2" s="6">
-        <v>3.9430000000000001</v>
-      </c>
-      <c r="IZ2" s="6">
-        <v>3.98</v>
-      </c>
-      <c r="JA2" s="6">
-        <v>4.375</v>
-      </c>
-      <c r="JB2" s="6">
-        <v>4.5110000000000001</v>
-      </c>
-      <c r="JC2" s="6">
-        <v>4.8360000000000003</v>
-      </c>
-      <c r="JD2" s="6">
-        <v>4.7949999999999999</v>
-      </c>
-      <c r="JE2" s="6">
-        <v>4.2990000000000004</v>
-      </c>
-      <c r="JF2" s="6">
-        <v>4.2130000000000001</v>
-      </c>
-      <c r="JG2" s="6">
-        <v>3.923</v>
-      </c>
-      <c r="JH2" s="6">
-        <v>3.8719999999999999</v>
-      </c>
-      <c r="JI2" s="6">
-        <v>3.7879999999999998</v>
-      </c>
-      <c r="JJ2" s="6">
-        <v>3.758</v>
-      </c>
-      <c r="JK2" s="6">
-        <v>3.9079999999999999</v>
-      </c>
-      <c r="JL2" s="6">
-        <v>4.0259999999999998</v>
-      </c>
-      <c r="JM2" s="6">
-        <v>4.3579999999999997</v>
-      </c>
-      <c r="JN2" s="6">
-        <v>4.5759999999999996</v>
-      </c>
-      <c r="JO2" s="6">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="JP2" s="6">
-        <v>4.7880000000000003</v>
-      </c>
-      <c r="JQ2" s="6">
-        <v>4.3220000000000001</v>
-      </c>
-      <c r="JR2" s="6">
-        <v>4.3410000000000002</v>
-      </c>
-      <c r="JS2" s="6">
-        <v>3.8740000000000001</v>
-      </c>
-      <c r="JT2" s="6">
-        <v>3.9220000000000002</v>
-      </c>
-      <c r="JU2" s="6">
-        <v>3.7770000000000001</v>
-      </c>
-      <c r="JV2" s="6">
-        <v>3.7080000000000002</v>
-      </c>
-      <c r="JW2" s="6">
-        <v>4.0119999999999996</v>
-      </c>
-      <c r="JX2" s="6">
-        <v>3.97</v>
-      </c>
-      <c r="JY2" s="6">
-        <v>4.3479999999999999</v>
-      </c>
-      <c r="JZ2" s="6">
-        <v>4.4450000000000003</v>
-      </c>
       <c r="KA2" s="6">
-        <v>4.8099999999999996</v>
+        <v>4.2649999999999997</v>
       </c>
       <c r="KB2" s="6">
         <v>4.8230000000000004</v>

</xml_diff>